<commit_message>
Finished results reporting and added optional plots per job to show travel path
</commit_message>
<xml_diff>
--- a/input/test_1/setup.xlsx
+++ b/input/test_1/setup.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sam.secher\source\repos\pnp-opt\input\test_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76F7595F-FF94-4910-98F4-E531625D4384}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E32AA967-B6A0-400E-B32B-FFA185B68CBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="3" xr2:uid="{44D22B83-19E5-49DB-9A86-332D4007F8A2}"/>
   </bookViews>
@@ -536,7 +536,7 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -618,7 +618,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -746,7 +746,7 @@
   <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Fixed placement model results reporting to correctly handle values that are very close to 0 or 1. Also fixed double counting of place and vision align time.
</commit_message>
<xml_diff>
--- a/input/test_1/setup.xlsx
+++ b/input/test_1/setup.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sam.secher\source\repos\pnp-opt\input\test_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E32AA967-B6A0-400E-B32B-FFA185B68CBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B79987D4-2B4F-4BA8-8935-F8FEA79FDE02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="3" xr2:uid="{44D22B83-19E5-49DB-9A86-332D4007F8A2}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{44D22B83-19E5-49DB-9A86-332D4007F8A2}"/>
   </bookViews>
   <sheets>
     <sheet name="machine" sheetId="1" r:id="rId1"/>
@@ -535,8 +535,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BAFECAB-9894-4316-8F2A-02B6AAA65DCF}">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -573,7 +573,7 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>500</v>
+        <v>100</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
@@ -745,7 +745,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB3C4590-047C-4F14-9E24-EF18F41AFAFA}">
   <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>

</xml_diff>